<commit_message>
Minor changes to data
Removed 'BX98 Rikers Island1' because no work force. Changed 'MN01 Marble Hill2-Inwood' to remove the number
</commit_message>
<xml_diff>
--- a/Personal_Fit_Model/nyc_race.xlsx
+++ b/Personal_Fit_Model/nyc_race.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\realtor-insights\Personal_Fit_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D267DA2-73F9-42A9-A4A6-A23DCCF3A350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3122C3C5-51F4-4893-8115-FEB4EC39FD0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{164B5293-A9B7-4CCA-BF14-EAC43F3583AD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
   <si>
     <t>Total population</t>
   </si>
@@ -218,9 +218,6 @@
     <t>BX39 Mott Haven-Port Morris</t>
   </si>
   <si>
-    <t>BX98 Rikers Island</t>
-  </si>
-  <si>
     <t>BX01 Claremont-Bathgate</t>
   </si>
   <si>
@@ -395,30 +392,6 @@
     <t>MN34 East Harlem North</t>
   </si>
   <si>
-    <r>
-      <t>MN01 Marble Hill</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-Inwood</t>
-    </r>
-  </si>
-  <si>
     <t>MN35 Washington Heights North</t>
   </si>
   <si>
@@ -651,13 +624,16 @@
   </si>
   <si>
     <t>SI54 Great Kills</t>
+  </si>
+  <si>
+    <t>MN01 Marble Hill-Inwood</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,13 +661,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="superscript"/>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1061,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0817C2-49E6-4D9E-98A4-13019EE3A940}">
-  <dimension ref="A1:G194"/>
+  <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A198" sqref="A198"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,7 +1111,7 @@
         <v>2012</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G66" si="0">B3-C3-D3-E3-F3</f>
+        <f t="shared" ref="G3:G65" si="0">B3-C3-D3-E3-F3</f>
         <v>1142</v>
       </c>
     </row>
@@ -2423,23 +2392,23 @@
         <v>61</v>
       </c>
       <c r="B57" s="4">
-        <v>9741</v>
+        <v>30715</v>
       </c>
       <c r="C57" s="4">
-        <v>3304</v>
+        <v>17094</v>
       </c>
       <c r="D57" s="4">
-        <v>651</v>
+        <v>270</v>
       </c>
       <c r="E57" s="4">
-        <v>5484</v>
+        <v>12932</v>
       </c>
       <c r="F57" s="4">
-        <v>202</v>
+        <v>29</v>
       </c>
       <c r="G57" s="4">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2447,23 +2416,23 @@
         <v>62</v>
       </c>
       <c r="B58" s="4">
-        <v>30715</v>
+        <v>25783</v>
       </c>
       <c r="C58" s="4">
-        <v>17094</v>
+        <v>15391</v>
       </c>
       <c r="D58" s="4">
-        <v>270</v>
+        <v>4876</v>
       </c>
       <c r="E58" s="4">
-        <v>12932</v>
+        <v>4675</v>
       </c>
       <c r="F58" s="4">
-        <v>29</v>
+        <v>559</v>
       </c>
       <c r="G58" s="4">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>282</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -2471,23 +2440,23 @@
         <v>63</v>
       </c>
       <c r="B59" s="4">
-        <v>25783</v>
+        <v>41871</v>
       </c>
       <c r="C59" s="4">
-        <v>15391</v>
+        <v>29037</v>
       </c>
       <c r="D59" s="4">
-        <v>4876</v>
+        <v>916</v>
       </c>
       <c r="E59" s="4">
-        <v>4675</v>
+        <v>11252</v>
       </c>
       <c r="F59" s="4">
-        <v>559</v>
+        <v>337</v>
       </c>
       <c r="G59" s="4">
         <f t="shared" si="0"/>
-        <v>282</v>
+        <v>329</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -2495,23 +2464,23 @@
         <v>64</v>
       </c>
       <c r="B60" s="4">
-        <v>41871</v>
+        <v>37872</v>
       </c>
       <c r="C60" s="4">
-        <v>29037</v>
+        <v>23023</v>
       </c>
       <c r="D60" s="4">
-        <v>916</v>
+        <v>401</v>
       </c>
       <c r="E60" s="4">
-        <v>11252</v>
+        <v>13480</v>
       </c>
       <c r="F60" s="4">
-        <v>337</v>
+        <v>226</v>
       </c>
       <c r="G60" s="4">
         <f t="shared" si="0"/>
-        <v>329</v>
+        <v>742</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -2519,23 +2488,23 @@
         <v>65</v>
       </c>
       <c r="B61" s="4">
-        <v>37872</v>
+        <v>20352</v>
       </c>
       <c r="C61" s="4">
-        <v>23023</v>
+        <v>14588</v>
       </c>
       <c r="D61" s="4">
-        <v>401</v>
+        <v>247</v>
       </c>
       <c r="E61" s="4">
-        <v>13480</v>
+        <v>5037</v>
       </c>
       <c r="F61" s="4">
-        <v>226</v>
+        <v>129</v>
       </c>
       <c r="G61" s="4">
         <f t="shared" si="0"/>
-        <v>742</v>
+        <v>351</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -2543,23 +2512,23 @@
         <v>66</v>
       </c>
       <c r="B62" s="4">
-        <v>20352</v>
+        <v>63504</v>
       </c>
       <c r="C62" s="4">
-        <v>14588</v>
+        <v>36303</v>
       </c>
       <c r="D62" s="4">
-        <v>247</v>
+        <v>1140</v>
       </c>
       <c r="E62" s="4">
-        <v>5037</v>
+        <v>24376</v>
       </c>
       <c r="F62" s="4">
-        <v>129</v>
+        <v>623</v>
       </c>
       <c r="G62" s="4">
         <f t="shared" si="0"/>
-        <v>351</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -2567,23 +2536,23 @@
         <v>67</v>
       </c>
       <c r="B63" s="4">
-        <v>63504</v>
+        <v>37065</v>
       </c>
       <c r="C63" s="4">
-        <v>36303</v>
+        <v>23380</v>
       </c>
       <c r="D63" s="4">
-        <v>1140</v>
+        <v>237</v>
       </c>
       <c r="E63" s="4">
-        <v>24376</v>
+        <v>12997</v>
       </c>
       <c r="F63" s="4">
-        <v>623</v>
+        <v>158</v>
       </c>
       <c r="G63" s="4">
         <f t="shared" si="0"/>
-        <v>1062</v>
+        <v>293</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -2591,23 +2560,23 @@
         <v>68</v>
       </c>
       <c r="B64" s="4">
-        <v>37065</v>
+        <v>39680</v>
       </c>
       <c r="C64" s="4">
-        <v>23380</v>
+        <v>27766</v>
       </c>
       <c r="D64" s="4">
-        <v>237</v>
+        <v>886</v>
       </c>
       <c r="E64" s="4">
-        <v>12997</v>
+        <v>9464</v>
       </c>
       <c r="F64" s="4">
-        <v>158</v>
+        <v>928</v>
       </c>
       <c r="G64" s="4">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>636</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2615,23 +2584,23 @@
         <v>69</v>
       </c>
       <c r="B65" s="4">
-        <v>39680</v>
+        <v>53944</v>
       </c>
       <c r="C65" s="4">
-        <v>27766</v>
+        <v>35847</v>
       </c>
       <c r="D65" s="4">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="E65" s="4">
-        <v>9464</v>
+        <v>16243</v>
       </c>
       <c r="F65" s="4">
-        <v>928</v>
+        <v>294</v>
       </c>
       <c r="G65" s="4">
         <f t="shared" si="0"/>
-        <v>636</v>
+        <v>682</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2639,23 +2608,23 @@
         <v>70</v>
       </c>
       <c r="B66" s="4">
-        <v>53944</v>
+        <v>26336</v>
       </c>
       <c r="C66" s="4">
-        <v>35847</v>
+        <v>18064</v>
       </c>
       <c r="D66" s="4">
-        <v>878</v>
+        <v>403</v>
       </c>
       <c r="E66" s="4">
-        <v>16243</v>
+        <v>7468</v>
       </c>
       <c r="F66" s="4">
-        <v>294</v>
+        <v>171</v>
       </c>
       <c r="G66" s="4">
-        <f t="shared" si="0"/>
-        <v>682</v>
+        <f t="shared" ref="G66:G129" si="1">B66-C66-D66-E66-F66</f>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2663,23 +2632,23 @@
         <v>71</v>
       </c>
       <c r="B67" s="4">
-        <v>26336</v>
+        <v>52237</v>
       </c>
       <c r="C67" s="4">
-        <v>18064</v>
+        <v>35935</v>
       </c>
       <c r="D67" s="4">
-        <v>403</v>
+        <v>683</v>
       </c>
       <c r="E67" s="4">
-        <v>7468</v>
+        <v>13829</v>
       </c>
       <c r="F67" s="4">
-        <v>171</v>
+        <v>1128</v>
       </c>
       <c r="G67" s="4">
-        <f t="shared" ref="G67:G130" si="1">B67-C67-D67-E67-F67</f>
-        <v>230</v>
+        <f t="shared" si="1"/>
+        <v>662</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2687,23 +2656,23 @@
         <v>72</v>
       </c>
       <c r="B68" s="4">
-        <v>52237</v>
+        <v>52591</v>
       </c>
       <c r="C68" s="4">
-        <v>35935</v>
+        <v>35907</v>
       </c>
       <c r="D68" s="4">
-        <v>683</v>
+        <v>3981</v>
       </c>
       <c r="E68" s="4">
-        <v>13829</v>
+        <v>9408</v>
       </c>
       <c r="F68" s="4">
-        <v>1128</v>
+        <v>2516</v>
       </c>
       <c r="G68" s="4">
         <f t="shared" si="1"/>
-        <v>662</v>
+        <v>779</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -2711,23 +2680,23 @@
         <v>73</v>
       </c>
       <c r="B69" s="4">
-        <v>52591</v>
+        <v>30599</v>
       </c>
       <c r="C69" s="4">
-        <v>35907</v>
+        <v>20962</v>
       </c>
       <c r="D69" s="4">
-        <v>3981</v>
+        <v>850</v>
       </c>
       <c r="E69" s="4">
-        <v>9408</v>
+        <v>6242</v>
       </c>
       <c r="F69" s="4">
-        <v>2516</v>
+        <v>1999</v>
       </c>
       <c r="G69" s="4">
         <f t="shared" si="1"/>
-        <v>779</v>
+        <v>546</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2735,23 +2704,23 @@
         <v>74</v>
       </c>
       <c r="B70" s="4">
-        <v>30599</v>
+        <v>41217</v>
       </c>
       <c r="C70" s="4">
-        <v>20962</v>
+        <v>23125</v>
       </c>
       <c r="D70" s="4">
-        <v>850</v>
+        <v>5079</v>
       </c>
       <c r="E70" s="4">
-        <v>6242</v>
+        <v>8046</v>
       </c>
       <c r="F70" s="4">
-        <v>1999</v>
+        <v>3570</v>
       </c>
       <c r="G70" s="4">
         <f t="shared" si="1"/>
-        <v>546</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2759,23 +2728,23 @@
         <v>75</v>
       </c>
       <c r="B71" s="4">
-        <v>41217</v>
+        <v>26839</v>
       </c>
       <c r="C71" s="4">
-        <v>23125</v>
+        <v>4941</v>
       </c>
       <c r="D71" s="4">
-        <v>5079</v>
+        <v>17965</v>
       </c>
       <c r="E71" s="4">
-        <v>8046</v>
+        <v>1855</v>
       </c>
       <c r="F71" s="4">
-        <v>3570</v>
+        <v>1578</v>
       </c>
       <c r="G71" s="4">
         <f t="shared" si="1"/>
-        <v>1397</v>
+        <v>500</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -2783,23 +2752,23 @@
         <v>76</v>
       </c>
       <c r="B72" s="4">
-        <v>26839</v>
+        <v>49715</v>
       </c>
       <c r="C72" s="4">
-        <v>4941</v>
+        <v>31698</v>
       </c>
       <c r="D72" s="4">
-        <v>17965</v>
+        <v>5564</v>
       </c>
       <c r="E72" s="4">
-        <v>1855</v>
+        <v>9954</v>
       </c>
       <c r="F72" s="4">
-        <v>1578</v>
+        <v>1686</v>
       </c>
       <c r="G72" s="4">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>813</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -2807,23 +2776,23 @@
         <v>77</v>
       </c>
       <c r="B73" s="4">
-        <v>49715</v>
+        <v>29848</v>
       </c>
       <c r="C73" s="4">
-        <v>31698</v>
+        <v>10811</v>
       </c>
       <c r="D73" s="4">
-        <v>5564</v>
+        <v>14519</v>
       </c>
       <c r="E73" s="4">
-        <v>9954</v>
+        <v>1966</v>
       </c>
       <c r="F73" s="4">
-        <v>1686</v>
+        <v>1866</v>
       </c>
       <c r="G73" s="4">
         <f t="shared" si="1"/>
-        <v>813</v>
+        <v>686</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -2831,23 +2800,23 @@
         <v>78</v>
       </c>
       <c r="B74" s="4">
-        <v>29848</v>
+        <v>35325</v>
       </c>
       <c r="C74" s="4">
-        <v>10811</v>
+        <v>23944</v>
       </c>
       <c r="D74" s="4">
-        <v>14519</v>
+        <v>696</v>
       </c>
       <c r="E74" s="4">
-        <v>1966</v>
+        <v>8642</v>
       </c>
       <c r="F74" s="4">
-        <v>1866</v>
+        <v>937</v>
       </c>
       <c r="G74" s="4">
         <f t="shared" si="1"/>
-        <v>686</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -2855,23 +2824,23 @@
         <v>79</v>
       </c>
       <c r="B75" s="4">
-        <v>35325</v>
+        <v>53800</v>
       </c>
       <c r="C75" s="4">
-        <v>23944</v>
+        <v>33128</v>
       </c>
       <c r="D75" s="4">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="E75" s="4">
-        <v>8642</v>
+        <v>18304</v>
       </c>
       <c r="F75" s="4">
-        <v>937</v>
+        <v>883</v>
       </c>
       <c r="G75" s="4">
         <f t="shared" si="1"/>
-        <v>1106</v>
+        <v>797</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -2879,23 +2848,23 @@
         <v>80</v>
       </c>
       <c r="B76" s="4">
-        <v>53800</v>
+        <v>30376</v>
       </c>
       <c r="C76" s="4">
-        <v>33128</v>
+        <v>10749</v>
       </c>
       <c r="D76" s="4">
-        <v>688</v>
+        <v>1118</v>
       </c>
       <c r="E76" s="4">
-        <v>18304</v>
+        <v>14010</v>
       </c>
       <c r="F76" s="4">
-        <v>883</v>
+        <v>3746</v>
       </c>
       <c r="G76" s="4">
         <f t="shared" si="1"/>
-        <v>797</v>
+        <v>753</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -2903,23 +2872,23 @@
         <v>81</v>
       </c>
       <c r="B77" s="4">
-        <v>30376</v>
+        <v>35886</v>
       </c>
       <c r="C77" s="4">
-        <v>10749</v>
+        <v>23070</v>
       </c>
       <c r="D77" s="4">
-        <v>1118</v>
+        <v>597</v>
       </c>
       <c r="E77" s="4">
-        <v>14010</v>
+        <v>8066</v>
       </c>
       <c r="F77" s="4">
-        <v>3746</v>
+        <v>2567</v>
       </c>
       <c r="G77" s="4">
         <f t="shared" si="1"/>
-        <v>753</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -2927,23 +2896,23 @@
         <v>82</v>
       </c>
       <c r="B78" s="4">
-        <v>35886</v>
+        <v>27483</v>
       </c>
       <c r="C78" s="4">
-        <v>23070</v>
+        <v>16952</v>
       </c>
       <c r="D78" s="4">
-        <v>597</v>
+        <v>1542</v>
       </c>
       <c r="E78" s="4">
-        <v>8066</v>
+        <v>4076</v>
       </c>
       <c r="F78" s="4">
-        <v>2567</v>
+        <v>3992</v>
       </c>
       <c r="G78" s="4">
         <f t="shared" si="1"/>
-        <v>1586</v>
+        <v>921</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -2951,23 +2920,23 @@
         <v>83</v>
       </c>
       <c r="B79" s="4">
-        <v>27483</v>
+        <v>26139</v>
       </c>
       <c r="C79" s="4">
-        <v>16952</v>
+        <v>8201</v>
       </c>
       <c r="D79" s="4">
-        <v>1542</v>
+        <v>16180</v>
       </c>
       <c r="E79" s="4">
-        <v>4076</v>
+        <v>485</v>
       </c>
       <c r="F79" s="4">
-        <v>3992</v>
+        <v>905</v>
       </c>
       <c r="G79" s="4">
         <f t="shared" si="1"/>
-        <v>921</v>
+        <v>368</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -2975,23 +2944,23 @@
         <v>84</v>
       </c>
       <c r="B80" s="4">
-        <v>26139</v>
+        <v>44304</v>
       </c>
       <c r="C80" s="4">
-        <v>8201</v>
+        <v>12529</v>
       </c>
       <c r="D80" s="4">
-        <v>16180</v>
+        <v>3857</v>
       </c>
       <c r="E80" s="4">
-        <v>485</v>
+        <v>26996</v>
       </c>
       <c r="F80" s="4">
-        <v>905</v>
+        <v>521</v>
       </c>
       <c r="G80" s="4">
         <f t="shared" si="1"/>
-        <v>368</v>
+        <v>401</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -2999,23 +2968,23 @@
         <v>85</v>
       </c>
       <c r="B81" s="4">
-        <v>44304</v>
+        <v>46104</v>
       </c>
       <c r="C81" s="4">
-        <v>12529</v>
+        <v>18254</v>
       </c>
       <c r="D81" s="4">
-        <v>3857</v>
+        <v>21610</v>
       </c>
       <c r="E81" s="4">
-        <v>26996</v>
+        <v>3918</v>
       </c>
       <c r="F81" s="4">
-        <v>521</v>
+        <v>1091</v>
       </c>
       <c r="G81" s="4">
         <f t="shared" si="1"/>
-        <v>401</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3023,23 +2992,23 @@
         <v>86</v>
       </c>
       <c r="B82" s="4">
-        <v>46104</v>
+        <v>33728</v>
       </c>
       <c r="C82" s="4">
-        <v>18254</v>
+        <v>16914</v>
       </c>
       <c r="D82" s="4">
-        <v>21610</v>
+        <v>5023</v>
       </c>
       <c r="E82" s="4">
-        <v>3918</v>
+        <v>9781</v>
       </c>
       <c r="F82" s="4">
-        <v>1091</v>
+        <v>1401</v>
       </c>
       <c r="G82" s="4">
         <f t="shared" si="1"/>
-        <v>1231</v>
+        <v>609</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3047,23 +3016,23 @@
         <v>87</v>
       </c>
       <c r="B83" s="4">
-        <v>33728</v>
+        <v>33404</v>
       </c>
       <c r="C83" s="4">
-        <v>16914</v>
+        <v>9570</v>
       </c>
       <c r="D83" s="4">
-        <v>5023</v>
+        <v>9267</v>
       </c>
       <c r="E83" s="4">
-        <v>9781</v>
+        <v>10804</v>
       </c>
       <c r="F83" s="4">
-        <v>1401</v>
+        <v>3098</v>
       </c>
       <c r="G83" s="4">
         <f t="shared" si="1"/>
-        <v>609</v>
+        <v>665</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3071,23 +3040,23 @@
         <v>88</v>
       </c>
       <c r="B84" s="4">
-        <v>33404</v>
+        <v>30098</v>
       </c>
       <c r="C84" s="4">
-        <v>9570</v>
+        <v>16390</v>
       </c>
       <c r="D84" s="4">
-        <v>9267</v>
+        <v>7659</v>
       </c>
       <c r="E84" s="4">
-        <v>10804</v>
+        <v>2754</v>
       </c>
       <c r="F84" s="4">
-        <v>3098</v>
+        <v>2606</v>
       </c>
       <c r="G84" s="4">
         <f t="shared" si="1"/>
-        <v>665</v>
+        <v>689</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3095,23 +3064,23 @@
         <v>89</v>
       </c>
       <c r="B85" s="4">
-        <v>30098</v>
+        <v>30191</v>
       </c>
       <c r="C85" s="4">
-        <v>16390</v>
+        <v>11035</v>
       </c>
       <c r="D85" s="4">
-        <v>7659</v>
+        <v>11275</v>
       </c>
       <c r="E85" s="4">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="F85" s="4">
-        <v>2606</v>
+        <v>4496</v>
       </c>
       <c r="G85" s="4">
         <f t="shared" si="1"/>
-        <v>689</v>
+        <v>632</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3119,23 +3088,23 @@
         <v>90</v>
       </c>
       <c r="B86" s="4">
-        <v>30191</v>
+        <v>36676</v>
       </c>
       <c r="C86" s="4">
-        <v>11035</v>
+        <v>9050</v>
       </c>
       <c r="D86" s="4">
-        <v>11275</v>
+        <v>957</v>
       </c>
       <c r="E86" s="4">
-        <v>2753</v>
+        <v>25725</v>
       </c>
       <c r="F86" s="4">
-        <v>4496</v>
+        <v>372</v>
       </c>
       <c r="G86" s="4">
         <f t="shared" si="1"/>
-        <v>632</v>
+        <v>572</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3143,23 +3112,23 @@
         <v>91</v>
       </c>
       <c r="B87" s="4">
-        <v>36676</v>
+        <v>61503</v>
       </c>
       <c r="C87" s="4">
-        <v>9050</v>
+        <v>13502</v>
       </c>
       <c r="D87" s="4">
-        <v>957</v>
+        <v>1455</v>
       </c>
       <c r="E87" s="4">
-        <v>25725</v>
+        <v>44076</v>
       </c>
       <c r="F87" s="4">
-        <v>372</v>
+        <v>989</v>
       </c>
       <c r="G87" s="4">
         <f t="shared" si="1"/>
-        <v>572</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3167,23 +3136,23 @@
         <v>92</v>
       </c>
       <c r="B88" s="4">
-        <v>61503</v>
+        <v>45805</v>
       </c>
       <c r="C88" s="4">
-        <v>13502</v>
+        <v>7130</v>
       </c>
       <c r="D88" s="4">
-        <v>1455</v>
+        <v>7496</v>
       </c>
       <c r="E88" s="4">
-        <v>44076</v>
+        <v>28752</v>
       </c>
       <c r="F88" s="4">
-        <v>989</v>
+        <v>1546</v>
       </c>
       <c r="G88" s="4">
         <f t="shared" si="1"/>
-        <v>1481</v>
+        <v>881</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3191,23 +3160,23 @@
         <v>93</v>
       </c>
       <c r="B89" s="4">
-        <v>45805</v>
+        <v>1377</v>
       </c>
       <c r="C89" s="4">
-        <v>7130</v>
+        <v>789</v>
       </c>
       <c r="D89" s="4">
-        <v>7496</v>
+        <v>110</v>
       </c>
       <c r="E89" s="4">
-        <v>28752</v>
+        <v>389</v>
       </c>
       <c r="F89" s="4">
-        <v>1546</v>
+        <v>89</v>
       </c>
       <c r="G89" s="4">
         <f t="shared" si="1"/>
-        <v>881</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3215,23 +3184,23 @@
         <v>94</v>
       </c>
       <c r="B90" s="4">
-        <v>1377</v>
+        <v>67185</v>
       </c>
       <c r="C90" s="4">
-        <v>789</v>
+        <v>3908</v>
       </c>
       <c r="D90" s="4">
-        <v>110</v>
+        <v>54147</v>
       </c>
       <c r="E90" s="4">
-        <v>389</v>
+        <v>1133</v>
       </c>
       <c r="F90" s="4">
-        <v>89</v>
+        <v>5766</v>
       </c>
       <c r="G90" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3239,23 +3208,23 @@
         <v>95</v>
       </c>
       <c r="B91" s="4">
-        <v>67185</v>
+        <v>40059</v>
       </c>
       <c r="C91" s="4">
-        <v>3908</v>
+        <v>2188</v>
       </c>
       <c r="D91" s="4">
-        <v>54147</v>
+        <v>26345</v>
       </c>
       <c r="E91" s="4">
-        <v>1133</v>
+        <v>854</v>
       </c>
       <c r="F91" s="4">
-        <v>5766</v>
+        <v>9310</v>
       </c>
       <c r="G91" s="4">
         <f t="shared" si="1"/>
-        <v>2231</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3263,23 +3232,23 @@
         <v>96</v>
       </c>
       <c r="B92" s="4">
-        <v>40059</v>
+        <v>37506</v>
       </c>
       <c r="C92" s="4">
-        <v>2188</v>
+        <v>3623</v>
       </c>
       <c r="D92" s="4">
-        <v>26345</v>
+        <v>24524</v>
       </c>
       <c r="E92" s="4">
-        <v>854</v>
+        <v>1107</v>
       </c>
       <c r="F92" s="4">
-        <v>9310</v>
+        <v>7120</v>
       </c>
       <c r="G92" s="4">
         <f t="shared" si="1"/>
-        <v>1362</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3287,23 +3256,23 @@
         <v>97</v>
       </c>
       <c r="B93" s="4">
-        <v>37506</v>
+        <v>43755</v>
       </c>
       <c r="C93" s="4">
-        <v>3623</v>
+        <v>5195</v>
       </c>
       <c r="D93" s="4">
-        <v>24524</v>
+        <v>28595</v>
       </c>
       <c r="E93" s="4">
-        <v>1107</v>
+        <v>2456</v>
       </c>
       <c r="F93" s="4">
-        <v>7120</v>
+        <v>6341</v>
       </c>
       <c r="G93" s="4">
         <f t="shared" si="1"/>
-        <v>1132</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3311,23 +3280,23 @@
         <v>98</v>
       </c>
       <c r="B94" s="4">
-        <v>43755</v>
+        <v>46550</v>
       </c>
       <c r="C94" s="4">
-        <v>5195</v>
+        <v>5918</v>
       </c>
       <c r="D94" s="4">
-        <v>28595</v>
+        <v>7385</v>
       </c>
       <c r="E94" s="4">
-        <v>2456</v>
+        <v>1837</v>
       </c>
       <c r="F94" s="4">
-        <v>6341</v>
+        <v>30032</v>
       </c>
       <c r="G94" s="4">
         <f t="shared" si="1"/>
-        <v>1168</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3335,23 +3304,23 @@
         <v>99</v>
       </c>
       <c r="B95" s="4">
-        <v>46550</v>
+        <v>74243</v>
       </c>
       <c r="C95" s="4">
-        <v>5918</v>
+        <v>28817</v>
       </c>
       <c r="D95" s="4">
-        <v>7385</v>
+        <v>17709</v>
       </c>
       <c r="E95" s="4">
-        <v>1837</v>
+        <v>6596</v>
       </c>
       <c r="F95" s="4">
-        <v>30032</v>
+        <v>19151</v>
       </c>
       <c r="G95" s="4">
         <f t="shared" si="1"/>
-        <v>1378</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -3359,23 +3328,23 @@
         <v>100</v>
       </c>
       <c r="B96" s="4">
-        <v>74243</v>
+        <v>69299</v>
       </c>
       <c r="C96" s="4">
-        <v>28817</v>
+        <v>10649</v>
       </c>
       <c r="D96" s="4">
-        <v>17709</v>
+        <v>44507</v>
       </c>
       <c r="E96" s="4">
-        <v>6596</v>
+        <v>3589</v>
       </c>
       <c r="F96" s="4">
-        <v>19151</v>
+        <v>8210</v>
       </c>
       <c r="G96" s="4">
         <f t="shared" si="1"/>
-        <v>1970</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -3383,23 +3352,23 @@
         <v>101</v>
       </c>
       <c r="B97" s="4">
-        <v>69299</v>
+        <v>42931</v>
       </c>
       <c r="C97" s="4">
-        <v>10649</v>
+        <v>8669</v>
       </c>
       <c r="D97" s="4">
-        <v>44507</v>
+        <v>24858</v>
       </c>
       <c r="E97" s="4">
-        <v>3589</v>
+        <v>2560</v>
       </c>
       <c r="F97" s="4">
-        <v>8210</v>
+        <v>5841</v>
       </c>
       <c r="G97" s="4">
         <f t="shared" si="1"/>
-        <v>2344</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -3407,23 +3376,23 @@
         <v>102</v>
       </c>
       <c r="B98" s="4">
-        <v>42931</v>
+        <v>28228</v>
       </c>
       <c r="C98" s="4">
-        <v>8669</v>
+        <v>2009</v>
       </c>
       <c r="D98" s="4">
-        <v>24858</v>
+        <v>19251</v>
       </c>
       <c r="E98" s="4">
-        <v>2560</v>
+        <v>1180</v>
       </c>
       <c r="F98" s="4">
-        <v>5841</v>
+        <v>4905</v>
       </c>
       <c r="G98" s="4">
         <f t="shared" si="1"/>
-        <v>1003</v>
+        <v>883</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -3431,23 +3400,23 @@
         <v>103</v>
       </c>
       <c r="B99" s="4">
-        <v>28228</v>
+        <v>48393</v>
       </c>
       <c r="C99" s="4">
-        <v>2009</v>
+        <v>2903</v>
       </c>
       <c r="D99" s="4">
-        <v>19251</v>
+        <v>36720</v>
       </c>
       <c r="E99" s="4">
-        <v>1180</v>
+        <v>1030</v>
       </c>
       <c r="F99" s="4">
-        <v>4905</v>
+        <v>6884</v>
       </c>
       <c r="G99" s="4">
         <f t="shared" si="1"/>
-        <v>883</v>
+        <v>856</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -3455,23 +3424,23 @@
         <v>104</v>
       </c>
       <c r="B100" s="4">
-        <v>48393</v>
+        <v>49515</v>
       </c>
       <c r="C100" s="4">
-        <v>2903</v>
+        <v>5024</v>
       </c>
       <c r="D100" s="4">
-        <v>36720</v>
+        <v>34525</v>
       </c>
       <c r="E100" s="4">
-        <v>1030</v>
+        <v>2137</v>
       </c>
       <c r="F100" s="4">
-        <v>6884</v>
+        <v>6827</v>
       </c>
       <c r="G100" s="4">
         <f t="shared" si="1"/>
-        <v>856</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -3479,23 +3448,23 @@
         <v>105</v>
       </c>
       <c r="B101" s="4">
-        <v>49515</v>
+        <v>26075</v>
       </c>
       <c r="C101" s="4">
-        <v>5024</v>
+        <v>1682</v>
       </c>
       <c r="D101" s="4">
-        <v>34525</v>
+        <v>20151</v>
       </c>
       <c r="E101" s="4">
-        <v>2137</v>
+        <v>699</v>
       </c>
       <c r="F101" s="4">
-        <v>6827</v>
+        <v>2849</v>
       </c>
       <c r="G101" s="4">
         <f t="shared" si="1"/>
-        <v>1002</v>
+        <v>694</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -3503,23 +3472,23 @@
         <v>106</v>
       </c>
       <c r="B102" s="4">
-        <v>26075</v>
+        <v>21864</v>
       </c>
       <c r="C102" s="4">
-        <v>1682</v>
+        <v>1311</v>
       </c>
       <c r="D102" s="4">
-        <v>20151</v>
+        <v>15347</v>
       </c>
       <c r="E102" s="4">
-        <v>699</v>
+        <v>1076</v>
       </c>
       <c r="F102" s="4">
-        <v>2849</v>
+        <v>3593</v>
       </c>
       <c r="G102" s="4">
         <f t="shared" si="1"/>
-        <v>694</v>
+        <v>537</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -3527,23 +3496,23 @@
         <v>107</v>
       </c>
       <c r="B103" s="4">
-        <v>21864</v>
+        <v>135718</v>
       </c>
       <c r="C103" s="4">
-        <v>1311</v>
+        <v>20255</v>
       </c>
       <c r="D103" s="4">
-        <v>15347</v>
+        <v>92083</v>
       </c>
       <c r="E103" s="4">
-        <v>1076</v>
+        <v>11307</v>
       </c>
       <c r="F103" s="4">
-        <v>3593</v>
+        <v>8638</v>
       </c>
       <c r="G103" s="4">
         <f t="shared" si="1"/>
-        <v>537</v>
+        <v>3435</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -3551,23 +3520,23 @@
         <v>108</v>
       </c>
       <c r="B104" s="4">
-        <v>135718</v>
+        <v>60205</v>
       </c>
       <c r="C104" s="4">
-        <v>20255</v>
+        <v>6563</v>
       </c>
       <c r="D104" s="4">
-        <v>92083</v>
+        <v>43803</v>
       </c>
       <c r="E104" s="4">
-        <v>11307</v>
+        <v>1981</v>
       </c>
       <c r="F104" s="4">
-        <v>8638</v>
+        <v>6364</v>
       </c>
       <c r="G104" s="4">
         <f t="shared" si="1"/>
-        <v>3435</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -3575,23 +3544,23 @@
         <v>109</v>
       </c>
       <c r="B105" s="4">
-        <v>60205</v>
+        <v>81378</v>
       </c>
       <c r="C105" s="4">
-        <v>6563</v>
+        <v>5788</v>
       </c>
       <c r="D105" s="4">
-        <v>43803</v>
+        <v>61401</v>
       </c>
       <c r="E105" s="4">
-        <v>1981</v>
+        <v>3559</v>
       </c>
       <c r="F105" s="4">
-        <v>6364</v>
+        <v>8720</v>
       </c>
       <c r="G105" s="4">
         <f t="shared" si="1"/>
-        <v>1494</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -3599,23 +3568,23 @@
         <v>110</v>
       </c>
       <c r="B106" s="4">
-        <v>81378</v>
+        <v>77676</v>
       </c>
       <c r="C106" s="4">
-        <v>5788</v>
+        <v>7105</v>
       </c>
       <c r="D106" s="4">
-        <v>61401</v>
+        <v>59737</v>
       </c>
       <c r="E106" s="4">
-        <v>3559</v>
+        <v>2329</v>
       </c>
       <c r="F106" s="4">
-        <v>8720</v>
+        <v>7034</v>
       </c>
       <c r="G106" s="4">
         <f t="shared" si="1"/>
-        <v>1910</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -3623,23 +3592,23 @@
         <v>111</v>
       </c>
       <c r="B107" s="4">
-        <v>77676</v>
+        <v>58834</v>
       </c>
       <c r="C107" s="4">
-        <v>7105</v>
+        <v>2938</v>
       </c>
       <c r="D107" s="4">
-        <v>59737</v>
+        <v>50878</v>
       </c>
       <c r="E107" s="4">
-        <v>2329</v>
+        <v>769</v>
       </c>
       <c r="F107" s="4">
-        <v>7034</v>
+        <v>3150</v>
       </c>
       <c r="G107" s="4">
         <f t="shared" si="1"/>
-        <v>1471</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -3647,23 +3616,23 @@
         <v>112</v>
       </c>
       <c r="B108" s="4">
-        <v>58834</v>
+        <v>51527</v>
       </c>
       <c r="C108" s="4">
-        <v>2938</v>
+        <v>25515</v>
       </c>
       <c r="D108" s="4">
-        <v>50878</v>
+        <v>6517</v>
       </c>
       <c r="E108" s="4">
-        <v>769</v>
+        <v>17246</v>
       </c>
       <c r="F108" s="4">
-        <v>3150</v>
+        <v>789</v>
       </c>
       <c r="G108" s="4">
         <f t="shared" si="1"/>
-        <v>1099</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -3671,23 +3640,23 @@
         <v>113</v>
       </c>
       <c r="B109" s="4">
-        <v>51527</v>
+        <v>23845</v>
       </c>
       <c r="C109" s="4">
-        <v>25515</v>
+        <v>13312</v>
       </c>
       <c r="D109" s="4">
-        <v>6517</v>
+        <v>2097</v>
       </c>
       <c r="E109" s="4">
-        <v>17246</v>
+        <v>6911</v>
       </c>
       <c r="F109" s="4">
-        <v>789</v>
+        <v>839</v>
       </c>
       <c r="G109" s="4">
         <f t="shared" si="1"/>
-        <v>1460</v>
+        <v>686</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -3695,23 +3664,23 @@
         <v>114</v>
       </c>
       <c r="B110" s="4">
-        <v>23845</v>
+        <v>54326</v>
       </c>
       <c r="C110" s="4">
-        <v>13312</v>
+        <v>12360</v>
       </c>
       <c r="D110" s="4">
-        <v>2097</v>
+        <v>26036</v>
       </c>
       <c r="E110" s="4">
-        <v>6911</v>
+        <v>6349</v>
       </c>
       <c r="F110" s="4">
-        <v>839</v>
+        <v>7783</v>
       </c>
       <c r="G110" s="4">
         <f t="shared" si="1"/>
-        <v>686</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -3719,23 +3688,23 @@
         <v>115</v>
       </c>
       <c r="B111" s="4">
-        <v>54326</v>
+        <v>78193</v>
       </c>
       <c r="C111" s="4">
-        <v>12360</v>
+        <v>17786</v>
       </c>
       <c r="D111" s="4">
-        <v>26036</v>
+        <v>5941</v>
       </c>
       <c r="E111" s="4">
-        <v>6349</v>
+        <v>49878</v>
       </c>
       <c r="F111" s="4">
-        <v>7783</v>
+        <v>2082</v>
       </c>
       <c r="G111" s="4">
         <f t="shared" si="1"/>
-        <v>1798</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -3743,23 +3712,23 @@
         <v>116</v>
       </c>
       <c r="B112" s="4">
-        <v>78193</v>
+        <v>46694</v>
       </c>
       <c r="C112" s="4">
-        <v>17786</v>
+        <v>8793</v>
       </c>
       <c r="D112" s="4">
-        <v>5941</v>
+        <v>8324</v>
       </c>
       <c r="E112" s="4">
-        <v>49878</v>
+        <v>26420</v>
       </c>
       <c r="F112" s="4">
-        <v>2082</v>
+        <v>1809</v>
       </c>
       <c r="G112" s="4">
         <f t="shared" si="1"/>
-        <v>2506</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
@@ -3767,23 +3736,23 @@
         <v>117</v>
       </c>
       <c r="B113" s="4">
-        <v>46694</v>
+        <v>59794</v>
       </c>
       <c r="C113" s="4">
-        <v>8793</v>
+        <v>26328</v>
       </c>
       <c r="D113" s="4">
-        <v>8324</v>
+        <v>11085</v>
       </c>
       <c r="E113" s="4">
-        <v>26420</v>
+        <v>15029</v>
       </c>
       <c r="F113" s="4">
-        <v>1809</v>
+        <v>5932</v>
       </c>
       <c r="G113" s="4">
         <f t="shared" si="1"/>
-        <v>1348</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -3791,1942 +3760,1918 @@
         <v>118</v>
       </c>
       <c r="B114" s="4">
-        <v>59794</v>
+        <v>60465</v>
       </c>
       <c r="C114" s="4">
-        <v>26328</v>
+        <v>31253</v>
       </c>
       <c r="D114" s="4">
-        <v>11085</v>
+        <v>5087</v>
       </c>
       <c r="E114" s="4">
-        <v>15029</v>
+        <v>21066</v>
       </c>
       <c r="F114" s="4">
-        <v>5932</v>
+        <v>2190</v>
       </c>
       <c r="G114" s="4">
         <f t="shared" si="1"/>
-        <v>1420</v>
+        <v>869</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>119</v>
+        <v>197</v>
       </c>
       <c r="B115" s="4">
-        <v>60465</v>
+        <v>50358</v>
       </c>
       <c r="C115" s="4">
-        <v>31253</v>
+        <v>37889</v>
       </c>
       <c r="D115" s="4">
-        <v>5087</v>
+        <v>6909</v>
       </c>
       <c r="E115" s="4">
-        <v>21066</v>
+        <v>3884</v>
       </c>
       <c r="F115" s="4">
-        <v>2190</v>
+        <v>652</v>
       </c>
       <c r="G115" s="4">
         <f t="shared" si="1"/>
-        <v>869</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B116" s="4">
-        <v>50358</v>
+        <v>71085</v>
       </c>
       <c r="C116" s="4">
-        <v>37889</v>
+        <v>46510</v>
       </c>
       <c r="D116" s="4">
-        <v>6909</v>
+        <v>18415</v>
       </c>
       <c r="E116" s="4">
-        <v>3884</v>
+        <v>3330</v>
       </c>
       <c r="F116" s="4">
-        <v>652</v>
+        <v>2032</v>
       </c>
       <c r="G116" s="4">
         <f t="shared" si="1"/>
-        <v>1024</v>
+        <v>798</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B117" s="4">
-        <v>71085</v>
+        <v>89551</v>
       </c>
       <c r="C117" s="4">
-        <v>46510</v>
+        <v>64553</v>
       </c>
       <c r="D117" s="4">
-        <v>18415</v>
+        <v>9699</v>
       </c>
       <c r="E117" s="4">
-        <v>3330</v>
+        <v>10853</v>
       </c>
       <c r="F117" s="4">
-        <v>2032</v>
+        <v>2445</v>
       </c>
       <c r="G117" s="4">
         <f t="shared" si="1"/>
-        <v>798</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B118" s="4">
-        <v>89551</v>
+        <v>1483</v>
       </c>
       <c r="C118" s="4">
-        <v>64553</v>
+        <v>454</v>
       </c>
       <c r="D118" s="4">
-        <v>9699</v>
+        <v>245</v>
       </c>
       <c r="E118" s="4">
-        <v>10853</v>
+        <v>747</v>
       </c>
       <c r="F118" s="4">
-        <v>2445</v>
+        <v>6</v>
       </c>
       <c r="G118" s="4">
         <f t="shared" si="1"/>
-        <v>2001</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B119" s="4">
-        <v>1483</v>
+        <v>18539</v>
       </c>
       <c r="C119" s="4">
-        <v>454</v>
+        <v>8128</v>
       </c>
       <c r="D119" s="4">
-        <v>245</v>
+        <v>3347</v>
       </c>
       <c r="E119" s="4">
-        <v>747</v>
+        <v>4179</v>
       </c>
       <c r="F119" s="4">
-        <v>6</v>
+        <v>2454</v>
       </c>
       <c r="G119" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>431</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B120" s="4">
-        <v>18539</v>
+        <v>75149</v>
       </c>
       <c r="C120" s="4">
-        <v>8128</v>
+        <v>21277</v>
       </c>
       <c r="D120" s="4">
-        <v>3347</v>
+        <v>38555</v>
       </c>
       <c r="E120" s="4">
-        <v>4179</v>
+        <v>3511</v>
       </c>
       <c r="F120" s="4">
-        <v>2454</v>
+        <v>10109</v>
       </c>
       <c r="G120" s="4">
         <f t="shared" si="1"/>
-        <v>431</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B121" s="4">
-        <v>75149</v>
+        <v>26470</v>
       </c>
       <c r="C121" s="4">
-        <v>21277</v>
+        <v>8356</v>
       </c>
       <c r="D121" s="4">
-        <v>38555</v>
+        <v>10564</v>
       </c>
       <c r="E121" s="4">
-        <v>3511</v>
+        <v>2500</v>
       </c>
       <c r="F121" s="4">
-        <v>10109</v>
+        <v>4203</v>
       </c>
       <c r="G121" s="4">
         <f t="shared" si="1"/>
-        <v>1697</v>
+        <v>847</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B122" s="4">
-        <v>26470</v>
+        <v>49001</v>
       </c>
       <c r="C122" s="4">
-        <v>8356</v>
+        <v>10978</v>
       </c>
       <c r="D122" s="4">
-        <v>10564</v>
+        <v>31579</v>
       </c>
       <c r="E122" s="4">
-        <v>2500</v>
+        <v>951</v>
       </c>
       <c r="F122" s="4">
-        <v>4203</v>
+        <v>4471</v>
       </c>
       <c r="G122" s="4">
         <f t="shared" si="1"/>
-        <v>847</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B123" s="4">
-        <v>49001</v>
+        <v>438</v>
       </c>
       <c r="C123" s="4">
-        <v>10978</v>
+        <v>65</v>
       </c>
       <c r="D123" s="4">
-        <v>31579</v>
+        <v>210</v>
       </c>
       <c r="E123" s="4">
-        <v>951</v>
+        <v>60</v>
       </c>
       <c r="F123" s="4">
-        <v>4471</v>
+        <v>93</v>
       </c>
       <c r="G123" s="4">
         <f t="shared" si="1"/>
-        <v>1022</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B124" s="4">
-        <v>438</v>
+        <v>60575</v>
       </c>
       <c r="C124" s="4">
-        <v>65</v>
+        <v>21198</v>
       </c>
       <c r="D124" s="4">
-        <v>210</v>
+        <v>21650</v>
       </c>
       <c r="E124" s="4">
-        <v>60</v>
+        <v>1096</v>
       </c>
       <c r="F124" s="4">
-        <v>93</v>
+        <v>15301</v>
       </c>
       <c r="G124" s="4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B125" s="4">
-        <v>60575</v>
+        <v>25088</v>
       </c>
       <c r="C125" s="4">
-        <v>21198</v>
+        <v>6538</v>
       </c>
       <c r="D125" s="4">
-        <v>21650</v>
+        <v>3926</v>
       </c>
       <c r="E125" s="4">
-        <v>1096</v>
+        <v>135</v>
       </c>
       <c r="F125" s="4">
-        <v>15301</v>
+        <v>14270</v>
       </c>
       <c r="G125" s="4">
         <f t="shared" si="1"/>
-        <v>1330</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B126" s="4">
-        <v>25088</v>
+        <v>45259</v>
       </c>
       <c r="C126" s="4">
-        <v>6538</v>
+        <v>15533</v>
       </c>
       <c r="D126" s="4">
-        <v>3926</v>
+        <v>10897</v>
       </c>
       <c r="E126" s="4">
-        <v>135</v>
+        <v>778</v>
       </c>
       <c r="F126" s="4">
-        <v>14270</v>
+        <v>16914</v>
       </c>
       <c r="G126" s="4">
         <f t="shared" si="1"/>
-        <v>219</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B127" s="4">
-        <v>45259</v>
+        <v>50295</v>
       </c>
       <c r="C127" s="4">
-        <v>15533</v>
+        <v>43197</v>
       </c>
       <c r="D127" s="4">
-        <v>10897</v>
+        <v>664</v>
       </c>
       <c r="E127" s="4">
-        <v>778</v>
+        <v>1801</v>
       </c>
       <c r="F127" s="4">
-        <v>16914</v>
+        <v>4361</v>
       </c>
       <c r="G127" s="4">
         <f t="shared" si="1"/>
-        <v>1137</v>
+        <v>272</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B128" s="4">
-        <v>50295</v>
+        <v>23070</v>
       </c>
       <c r="C128" s="4">
-        <v>43197</v>
+        <v>14746</v>
       </c>
       <c r="D128" s="4">
-        <v>664</v>
+        <v>752</v>
       </c>
       <c r="E128" s="4">
-        <v>1801</v>
+        <v>5910</v>
       </c>
       <c r="F128" s="4">
-        <v>4361</v>
+        <v>1282</v>
       </c>
       <c r="G128" s="4">
         <f t="shared" si="1"/>
-        <v>272</v>
+        <v>380</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B129" s="4">
-        <v>23070</v>
+        <v>105188</v>
       </c>
       <c r="C129" s="4">
-        <v>14746</v>
+        <v>57031</v>
       </c>
       <c r="D129" s="4">
-        <v>752</v>
+        <v>17518</v>
       </c>
       <c r="E129" s="4">
-        <v>5910</v>
+        <v>2077</v>
       </c>
       <c r="F129" s="4">
-        <v>1282</v>
+        <v>25345</v>
       </c>
       <c r="G129" s="4">
         <f t="shared" si="1"/>
-        <v>380</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B130" s="4">
-        <v>105188</v>
+        <v>54091</v>
       </c>
       <c r="C130" s="4">
-        <v>57031</v>
+        <v>32553</v>
       </c>
       <c r="D130" s="4">
-        <v>17518</v>
+        <v>5124</v>
       </c>
       <c r="E130" s="4">
-        <v>2077</v>
+        <v>8078</v>
       </c>
       <c r="F130" s="4">
-        <v>25345</v>
+        <v>7750</v>
       </c>
       <c r="G130" s="4">
-        <f t="shared" si="1"/>
-        <v>3217</v>
+        <f t="shared" ref="G130:G192" si="2">B130-C130-D130-E130-F130</f>
+        <v>586</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B131" s="4">
-        <v>54091</v>
+        <v>84904</v>
       </c>
       <c r="C131" s="4">
-        <v>32553</v>
+        <v>38195</v>
       </c>
       <c r="D131" s="4">
-        <v>5124</v>
+        <v>5597</v>
       </c>
       <c r="E131" s="4">
-        <v>8078</v>
+        <v>953</v>
       </c>
       <c r="F131" s="4">
-        <v>7750</v>
+        <v>38892</v>
       </c>
       <c r="G131" s="4">
-        <f t="shared" ref="G131:G193" si="2">B131-C131-D131-E131-F131</f>
-        <v>586</v>
+        <f t="shared" si="2"/>
+        <v>1267</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B132" s="4">
-        <v>84904</v>
+        <v>31750</v>
       </c>
       <c r="C132" s="4">
-        <v>38195</v>
+        <v>11172</v>
       </c>
       <c r="D132" s="4">
-        <v>5597</v>
+        <v>18971</v>
       </c>
       <c r="E132" s="4">
-        <v>953</v>
+        <v>282</v>
       </c>
       <c r="F132" s="4">
-        <v>38892</v>
+        <v>938</v>
       </c>
       <c r="G132" s="4">
         <f t="shared" si="2"/>
-        <v>1267</v>
+        <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B133" s="4">
-        <v>31750</v>
+        <v>70166</v>
       </c>
       <c r="C133" s="4">
-        <v>11172</v>
+        <v>35863</v>
       </c>
       <c r="D133" s="4">
-        <v>18971</v>
+        <v>27067</v>
       </c>
       <c r="E133" s="4">
-        <v>282</v>
+        <v>1157</v>
       </c>
       <c r="F133" s="4">
-        <v>938</v>
+        <v>5442</v>
       </c>
       <c r="G133" s="4">
         <f t="shared" si="2"/>
-        <v>387</v>
+        <v>637</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B134" s="4">
-        <v>70166</v>
+        <v>39062</v>
       </c>
       <c r="C134" s="4">
-        <v>35863</v>
+        <v>6567</v>
       </c>
       <c r="D134" s="4">
-        <v>27067</v>
+        <v>29230</v>
       </c>
       <c r="E134" s="4">
-        <v>1157</v>
+        <v>372</v>
       </c>
       <c r="F134" s="4">
-        <v>5442</v>
+        <v>2637</v>
       </c>
       <c r="G134" s="4">
         <f t="shared" si="2"/>
-        <v>637</v>
+        <v>256</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B135" s="4">
-        <v>39062</v>
+        <v>27677</v>
       </c>
       <c r="C135" s="4">
-        <v>6567</v>
+        <v>7146</v>
       </c>
       <c r="D135" s="4">
-        <v>29230</v>
+        <v>17035</v>
       </c>
       <c r="E135" s="4">
-        <v>372</v>
+        <v>244</v>
       </c>
       <c r="F135" s="4">
-        <v>2637</v>
+        <v>2994</v>
       </c>
       <c r="G135" s="4">
         <f t="shared" si="2"/>
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B136" s="4">
-        <v>27677</v>
+        <v>84694</v>
       </c>
       <c r="C136" s="4">
-        <v>7146</v>
+        <v>10414</v>
       </c>
       <c r="D136" s="4">
-        <v>17035</v>
+        <v>49570</v>
       </c>
       <c r="E136" s="4">
-        <v>244</v>
+        <v>2165</v>
       </c>
       <c r="F136" s="4">
-        <v>2994</v>
+        <v>20625</v>
       </c>
       <c r="G136" s="4">
         <f t="shared" si="2"/>
-        <v>258</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B137" s="4">
-        <v>84694</v>
+        <v>27500</v>
       </c>
       <c r="C137" s="4">
-        <v>10414</v>
+        <v>4667</v>
       </c>
       <c r="D137" s="4">
-        <v>49570</v>
+        <v>12349</v>
       </c>
       <c r="E137" s="4">
-        <v>2165</v>
+        <v>683</v>
       </c>
       <c r="F137" s="4">
-        <v>20625</v>
+        <v>8787</v>
       </c>
       <c r="G137" s="4">
         <f t="shared" si="2"/>
-        <v>1920</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B138" s="4">
-        <v>27500</v>
+        <v>69382</v>
       </c>
       <c r="C138" s="4">
-        <v>4667</v>
+        <v>10939</v>
       </c>
       <c r="D138" s="4">
-        <v>12349</v>
+        <v>6613</v>
       </c>
       <c r="E138" s="4">
-        <v>683</v>
+        <v>2671</v>
       </c>
       <c r="F138" s="4">
-        <v>8787</v>
+        <v>46310</v>
       </c>
       <c r="G138" s="4">
         <f t="shared" si="2"/>
-        <v>1014</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B139" s="4">
-        <v>69382</v>
+        <v>24199</v>
       </c>
       <c r="C139" s="4">
-        <v>10939</v>
+        <v>8781</v>
       </c>
       <c r="D139" s="4">
-        <v>6613</v>
+        <v>7841</v>
       </c>
       <c r="E139" s="4">
-        <v>2671</v>
+        <v>546</v>
       </c>
       <c r="F139" s="4">
-        <v>46310</v>
+        <v>6486</v>
       </c>
       <c r="G139" s="4">
         <f t="shared" si="2"/>
-        <v>2849</v>
+        <v>545</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B140" s="4">
-        <v>24199</v>
+        <v>22943</v>
       </c>
       <c r="C140" s="4">
-        <v>8781</v>
+        <v>2142</v>
       </c>
       <c r="D140" s="4">
-        <v>7841</v>
+        <v>14619</v>
       </c>
       <c r="E140" s="4">
-        <v>546</v>
+        <v>147</v>
       </c>
       <c r="F140" s="4">
-        <v>6486</v>
+        <v>5742</v>
       </c>
       <c r="G140" s="4">
         <f t="shared" si="2"/>
-        <v>545</v>
+        <v>293</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B141" s="4">
-        <v>22943</v>
+        <v>32331</v>
       </c>
       <c r="C141" s="4">
-        <v>2142</v>
+        <v>4701</v>
       </c>
       <c r="D141" s="4">
-        <v>14619</v>
+        <v>22016</v>
       </c>
       <c r="E141" s="4">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="F141" s="4">
-        <v>5742</v>
+        <v>4983</v>
       </c>
       <c r="G141" s="4">
         <f t="shared" si="2"/>
-        <v>293</v>
+        <v>463</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B142" s="4">
-        <v>32331</v>
+        <v>51509</v>
       </c>
       <c r="C142" s="4">
-        <v>4701</v>
+        <v>7766</v>
       </c>
       <c r="D142" s="4">
-        <v>22016</v>
+        <v>13982</v>
       </c>
       <c r="E142" s="4">
-        <v>168</v>
+        <v>764</v>
       </c>
       <c r="F142" s="4">
-        <v>4983</v>
+        <v>27903</v>
       </c>
       <c r="G142" s="4">
         <f t="shared" si="2"/>
-        <v>463</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B143" s="4">
-        <v>51509</v>
+        <v>27943</v>
       </c>
       <c r="C143" s="4">
-        <v>7766</v>
+        <v>4318</v>
       </c>
       <c r="D143" s="4">
-        <v>13982</v>
+        <v>5951</v>
       </c>
       <c r="E143" s="4">
-        <v>764</v>
+        <v>426</v>
       </c>
       <c r="F143" s="4">
-        <v>27903</v>
+        <v>16334</v>
       </c>
       <c r="G143" s="4">
         <f t="shared" si="2"/>
-        <v>1094</v>
+        <v>914</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B144" s="4">
-        <v>27943</v>
+        <v>20989</v>
       </c>
       <c r="C144" s="4">
-        <v>4318</v>
+        <v>3072</v>
       </c>
       <c r="D144" s="4">
-        <v>5951</v>
+        <v>3561</v>
       </c>
       <c r="E144" s="4">
-        <v>426</v>
+        <v>319</v>
       </c>
       <c r="F144" s="4">
-        <v>16334</v>
+        <v>13347</v>
       </c>
       <c r="G144" s="4">
         <f t="shared" si="2"/>
-        <v>914</v>
+        <v>690</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B145" s="4">
-        <v>20989</v>
+        <v>25067</v>
       </c>
       <c r="C145" s="4">
-        <v>3072</v>
+        <v>3830</v>
       </c>
       <c r="D145" s="4">
-        <v>3561</v>
+        <v>6002</v>
       </c>
       <c r="E145" s="4">
-        <v>319</v>
+        <v>6456</v>
       </c>
       <c r="F145" s="4">
-        <v>13347</v>
+        <v>7569</v>
       </c>
       <c r="G145" s="4">
         <f t="shared" si="2"/>
-        <v>690</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B146" s="4">
-        <v>25067</v>
+        <v>38449</v>
       </c>
       <c r="C146" s="4">
-        <v>3830</v>
+        <v>9880</v>
       </c>
       <c r="D146" s="4">
-        <v>6002</v>
+        <v>8122</v>
       </c>
       <c r="E146" s="4">
-        <v>6456</v>
+        <v>4459</v>
       </c>
       <c r="F146" s="4">
-        <v>7569</v>
+        <v>13743</v>
       </c>
       <c r="G146" s="4">
         <f t="shared" si="2"/>
-        <v>1210</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B147" s="4">
-        <v>38449</v>
+        <v>36683</v>
       </c>
       <c r="C147" s="4">
-        <v>9880</v>
+        <v>4584</v>
       </c>
       <c r="D147" s="4">
-        <v>8122</v>
+        <v>19456</v>
       </c>
       <c r="E147" s="4">
-        <v>4459</v>
+        <v>3081</v>
       </c>
       <c r="F147" s="4">
-        <v>13743</v>
+        <v>8467</v>
       </c>
       <c r="G147" s="4">
         <f t="shared" si="2"/>
-        <v>2245</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B148" s="4">
-        <v>36683</v>
+        <v>33532</v>
       </c>
       <c r="C148" s="4">
-        <v>4584</v>
+        <v>6700</v>
       </c>
       <c r="D148" s="4">
-        <v>19456</v>
+        <v>11381</v>
       </c>
       <c r="E148" s="4">
-        <v>3081</v>
+        <v>3588</v>
       </c>
       <c r="F148" s="4">
-        <v>8467</v>
+        <v>10788</v>
       </c>
       <c r="G148" s="4">
         <f t="shared" si="2"/>
-        <v>1095</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B149" s="4">
-        <v>33532</v>
+        <v>18177</v>
       </c>
       <c r="C149" s="4">
-        <v>6700</v>
+        <v>2394</v>
       </c>
       <c r="D149" s="4">
-        <v>11381</v>
+        <v>5475</v>
       </c>
       <c r="E149" s="4">
-        <v>3588</v>
+        <v>688</v>
       </c>
       <c r="F149" s="4">
-        <v>10788</v>
+        <v>9127</v>
       </c>
       <c r="G149" s="4">
         <f t="shared" si="2"/>
-        <v>1075</v>
+        <v>493</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B150" s="4">
-        <v>18177</v>
+        <v>59550</v>
       </c>
       <c r="C150" s="4">
-        <v>2394</v>
+        <v>31359</v>
       </c>
       <c r="D150" s="4">
-        <v>5475</v>
+        <v>9744</v>
       </c>
       <c r="E150" s="4">
-        <v>688</v>
+        <v>3522</v>
       </c>
       <c r="F150" s="4">
-        <v>9127</v>
+        <v>13171</v>
       </c>
       <c r="G150" s="4">
         <f t="shared" si="2"/>
-        <v>493</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B151" s="4">
-        <v>59550</v>
+        <v>65199</v>
       </c>
       <c r="C151" s="4">
-        <v>31359</v>
+        <v>22785</v>
       </c>
       <c r="D151" s="4">
-        <v>9744</v>
+        <v>6721</v>
       </c>
       <c r="E151" s="4">
-        <v>3522</v>
+        <v>6072</v>
       </c>
       <c r="F151" s="4">
-        <v>13171</v>
+        <v>19447</v>
       </c>
       <c r="G151" s="4">
         <f t="shared" si="2"/>
-        <v>1754</v>
+        <v>10174</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B152" s="4">
-        <v>65199</v>
+        <v>22878</v>
       </c>
       <c r="C152" s="4">
-        <v>22785</v>
+        <v>6404</v>
       </c>
       <c r="D152" s="4">
-        <v>6721</v>
+        <v>10877</v>
       </c>
       <c r="E152" s="4">
-        <v>6072</v>
+        <v>1690</v>
       </c>
       <c r="F152" s="4">
-        <v>19447</v>
+        <v>3417</v>
       </c>
       <c r="G152" s="4">
         <f t="shared" si="2"/>
-        <v>10174</v>
+        <v>490</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B153" s="4">
-        <v>22878</v>
+        <v>80046</v>
       </c>
       <c r="C153" s="4">
-        <v>6404</v>
+        <v>17681</v>
       </c>
       <c r="D153" s="4">
-        <v>10877</v>
+        <v>5217</v>
       </c>
       <c r="E153" s="4">
-        <v>1690</v>
+        <v>18785</v>
       </c>
       <c r="F153" s="4">
-        <v>3417</v>
+        <v>19624</v>
       </c>
       <c r="G153" s="4">
         <f t="shared" si="2"/>
-        <v>490</v>
+        <v>18739</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B154" s="4">
-        <v>80046</v>
+        <v>22136</v>
       </c>
       <c r="C154" s="4">
-        <v>17681</v>
+        <v>9258</v>
       </c>
       <c r="D154" s="4">
-        <v>5217</v>
+        <v>6390</v>
       </c>
       <c r="E154" s="4">
-        <v>18785</v>
+        <v>1208</v>
       </c>
       <c r="F154" s="4">
-        <v>19624</v>
+        <v>4680</v>
       </c>
       <c r="G154" s="4">
         <f t="shared" si="2"/>
-        <v>18739</v>
+        <v>600</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B155" s="4">
-        <v>22136</v>
+        <v>28769</v>
       </c>
       <c r="C155" s="4">
-        <v>9258</v>
+        <v>6010</v>
       </c>
       <c r="D155" s="4">
-        <v>6390</v>
+        <v>21132</v>
       </c>
       <c r="E155" s="4">
-        <v>1208</v>
+        <v>430</v>
       </c>
       <c r="F155" s="4">
-        <v>4680</v>
+        <v>572</v>
       </c>
       <c r="G155" s="4">
         <f t="shared" si="2"/>
-        <v>600</v>
+        <v>625</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B156" s="4">
-        <v>28769</v>
+        <v>28097</v>
       </c>
       <c r="C156" s="4">
-        <v>6010</v>
+        <v>2117</v>
       </c>
       <c r="D156" s="4">
-        <v>21132</v>
+        <v>12563</v>
       </c>
       <c r="E156" s="4">
-        <v>430</v>
+        <v>463</v>
       </c>
       <c r="F156" s="4">
-        <v>572</v>
+        <v>12198</v>
       </c>
       <c r="G156" s="4">
         <f t="shared" si="2"/>
-        <v>625</v>
+        <v>756</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B157" s="4">
-        <v>28097</v>
+        <v>25619</v>
       </c>
       <c r="C157" s="4">
-        <v>2117</v>
+        <v>2812</v>
       </c>
       <c r="D157" s="4">
-        <v>12563</v>
+        <v>12649</v>
       </c>
       <c r="E157" s="4">
-        <v>463</v>
+        <v>678</v>
       </c>
       <c r="F157" s="4">
-        <v>12198</v>
+        <v>9383</v>
       </c>
       <c r="G157" s="4">
         <f t="shared" si="2"/>
-        <v>756</v>
+        <v>97</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B158" s="4">
-        <v>25619</v>
+        <v>45522</v>
       </c>
       <c r="C158" s="4">
-        <v>2812</v>
+        <v>6086</v>
       </c>
       <c r="D158" s="4">
-        <v>12649</v>
+        <v>21375</v>
       </c>
       <c r="E158" s="4">
-        <v>678</v>
+        <v>1112</v>
       </c>
       <c r="F158" s="4">
-        <v>9383</v>
+        <v>15390</v>
       </c>
       <c r="G158" s="4">
         <f t="shared" si="2"/>
-        <v>97</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B159" s="4">
-        <v>45522</v>
+        <v>20684</v>
       </c>
       <c r="C159" s="4">
-        <v>6086</v>
+        <v>2745</v>
       </c>
       <c r="D159" s="4">
-        <v>21375</v>
+        <v>8715</v>
       </c>
       <c r="E159" s="4">
-        <v>1112</v>
+        <v>164</v>
       </c>
       <c r="F159" s="4">
-        <v>15390</v>
+        <v>8605</v>
       </c>
       <c r="G159" s="4">
         <f t="shared" si="2"/>
-        <v>1559</v>
+        <v>455</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B160" s="4">
-        <v>20684</v>
+        <v>36864</v>
       </c>
       <c r="C160" s="4">
-        <v>2745</v>
+        <v>6240</v>
       </c>
       <c r="D160" s="4">
-        <v>8715</v>
+        <v>238</v>
       </c>
       <c r="E160" s="4">
-        <v>164</v>
+        <v>24897</v>
       </c>
       <c r="F160" s="4">
-        <v>8605</v>
+        <v>2320</v>
       </c>
       <c r="G160" s="4">
         <f t="shared" si="2"/>
-        <v>455</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B161" s="4">
-        <v>36864</v>
+        <v>26959</v>
       </c>
       <c r="C161" s="4">
-        <v>6240</v>
+        <v>1952</v>
       </c>
       <c r="D161" s="4">
-        <v>238</v>
+        <v>371</v>
       </c>
       <c r="E161" s="4">
-        <v>24897</v>
+        <v>24061</v>
       </c>
       <c r="F161" s="4">
-        <v>2320</v>
+        <v>454</v>
       </c>
       <c r="G161" s="4">
         <f t="shared" si="2"/>
-        <v>3169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B162" s="4">
-        <v>26959</v>
+        <v>21520</v>
       </c>
       <c r="C162" s="4">
-        <v>1952</v>
+        <v>2627</v>
       </c>
       <c r="D162" s="4">
-        <v>371</v>
+        <v>721</v>
       </c>
       <c r="E162" s="4">
-        <v>24061</v>
+        <v>13468</v>
       </c>
       <c r="F162" s="4">
-        <v>454</v>
+        <v>2766</v>
       </c>
       <c r="G162" s="4">
         <f t="shared" si="2"/>
-        <v>121</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B163" s="4">
-        <v>21520</v>
+        <v>51098</v>
       </c>
       <c r="C163" s="4">
-        <v>2627</v>
+        <v>3181</v>
       </c>
       <c r="D163" s="4">
-        <v>721</v>
+        <v>697</v>
       </c>
       <c r="E163" s="4">
-        <v>13468</v>
+        <v>45052</v>
       </c>
       <c r="F163" s="4">
-        <v>2766</v>
+        <v>760</v>
       </c>
       <c r="G163" s="4">
         <f t="shared" si="2"/>
-        <v>1938</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B164" s="4">
-        <v>51098</v>
+        <v>50922</v>
       </c>
       <c r="C164" s="4">
-        <v>3181</v>
+        <v>18959</v>
       </c>
       <c r="D164" s="4">
-        <v>697</v>
+        <v>1410</v>
       </c>
       <c r="E164" s="4">
-        <v>45052</v>
+        <v>10344</v>
       </c>
       <c r="F164" s="4">
-        <v>760</v>
+        <v>15383</v>
       </c>
       <c r="G164" s="4">
         <f t="shared" si="2"/>
-        <v>1408</v>
+        <v>4826</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B165" s="4">
-        <v>50922</v>
+        <v>34293</v>
       </c>
       <c r="C165" s="4">
-        <v>18959</v>
+        <v>3751</v>
       </c>
       <c r="D165" s="4">
-        <v>1410</v>
+        <v>199</v>
       </c>
       <c r="E165" s="4">
-        <v>10344</v>
+        <v>26638</v>
       </c>
       <c r="F165" s="4">
-        <v>15383</v>
+        <v>1531</v>
       </c>
       <c r="G165" s="4">
         <f t="shared" si="2"/>
-        <v>4826</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B166" s="4">
-        <v>34293</v>
+        <v>19901</v>
       </c>
       <c r="C166" s="4">
-        <v>3751</v>
+        <v>1590</v>
       </c>
       <c r="D166" s="4">
-        <v>199</v>
+        <v>384</v>
       </c>
       <c r="E166" s="4">
-        <v>26638</v>
+        <v>17185</v>
       </c>
       <c r="F166" s="4">
-        <v>1531</v>
+        <v>295</v>
       </c>
       <c r="G166" s="4">
         <f t="shared" si="2"/>
-        <v>2174</v>
+        <v>447</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B167" s="4">
-        <v>19901</v>
+        <v>28201</v>
       </c>
       <c r="C167" s="4">
-        <v>1590</v>
+        <v>1678</v>
       </c>
       <c r="D167" s="4">
-        <v>384</v>
+        <v>1172</v>
       </c>
       <c r="E167" s="4">
-        <v>17185</v>
+        <v>23768</v>
       </c>
       <c r="F167" s="4">
-        <v>295</v>
+        <v>1113</v>
       </c>
       <c r="G167" s="4">
         <f t="shared" si="2"/>
-        <v>447</v>
+        <v>470</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B168" s="4">
-        <v>28201</v>
+        <v>20212</v>
       </c>
       <c r="C168" s="4">
-        <v>1678</v>
+        <v>1026</v>
       </c>
       <c r="D168" s="4">
-        <v>1172</v>
+        <v>318</v>
       </c>
       <c r="E168" s="4">
-        <v>23768</v>
+        <v>18163</v>
       </c>
       <c r="F168" s="4">
-        <v>1113</v>
+        <v>423</v>
       </c>
       <c r="G168" s="4">
         <f t="shared" si="2"/>
-        <v>470</v>
+        <v>282</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B169" s="4">
-        <v>20212</v>
+        <v>57549</v>
       </c>
       <c r="C169" s="4">
-        <v>1026</v>
+        <v>10801</v>
       </c>
       <c r="D169" s="4">
-        <v>318</v>
+        <v>3227</v>
       </c>
       <c r="E169" s="4">
-        <v>18163</v>
+        <v>28682</v>
       </c>
       <c r="F169" s="4">
-        <v>423</v>
+        <v>10520</v>
       </c>
       <c r="G169" s="4">
         <f t="shared" si="2"/>
-        <v>282</v>
+        <v>4319</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B170" s="4">
-        <v>57549</v>
+        <v>25964</v>
       </c>
       <c r="C170" s="4">
-        <v>10801</v>
+        <v>3880</v>
       </c>
       <c r="D170" s="4">
-        <v>3227</v>
+        <v>9217</v>
       </c>
       <c r="E170" s="4">
-        <v>28682</v>
+        <v>1605</v>
       </c>
       <c r="F170" s="4">
-        <v>10520</v>
+        <v>10009</v>
       </c>
       <c r="G170" s="4">
         <f t="shared" si="2"/>
-        <v>4319</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B171" s="4">
-        <v>25964</v>
+        <v>22427</v>
       </c>
       <c r="C171" s="4">
-        <v>3880</v>
+        <v>2024</v>
       </c>
       <c r="D171" s="4">
-        <v>9217</v>
+        <v>11464</v>
       </c>
       <c r="E171" s="4">
-        <v>1605</v>
+        <v>663</v>
       </c>
       <c r="F171" s="4">
-        <v>10009</v>
+        <v>7181</v>
       </c>
       <c r="G171" s="4">
         <f t="shared" si="2"/>
-        <v>1253</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B172" s="4">
-        <v>22427</v>
+        <v>25141</v>
       </c>
       <c r="C172" s="4">
-        <v>2024</v>
+        <v>937</v>
       </c>
       <c r="D172" s="4">
-        <v>11464</v>
+        <v>406</v>
       </c>
       <c r="E172" s="4">
-        <v>663</v>
+        <v>23042</v>
       </c>
       <c r="F172" s="4">
-        <v>7181</v>
+        <v>97</v>
       </c>
       <c r="G172" s="4">
         <f t="shared" si="2"/>
-        <v>1095</v>
+        <v>659</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B173" s="4">
-        <v>25141</v>
+        <v>29543</v>
       </c>
       <c r="C173" s="4">
-        <v>937</v>
+        <v>3759</v>
       </c>
       <c r="D173" s="4">
-        <v>406</v>
+        <v>22907</v>
       </c>
       <c r="E173" s="4">
-        <v>23042</v>
+        <v>2104</v>
       </c>
       <c r="F173" s="4">
-        <v>97</v>
+        <v>453</v>
       </c>
       <c r="G173" s="4">
         <f t="shared" si="2"/>
-        <v>659</v>
+        <v>320</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B174" s="4">
-        <v>29543</v>
+        <v>35500</v>
       </c>
       <c r="C174" s="4">
-        <v>3759</v>
+        <v>9127</v>
       </c>
       <c r="D174" s="4">
-        <v>22907</v>
+        <v>4874</v>
       </c>
       <c r="E174" s="4">
-        <v>2104</v>
+        <v>19606</v>
       </c>
       <c r="F174" s="4">
-        <v>453</v>
+        <v>966</v>
       </c>
       <c r="G174" s="4">
         <f t="shared" si="2"/>
-        <v>320</v>
+        <v>927</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B175" s="4">
-        <v>35500</v>
+        <v>50294</v>
       </c>
       <c r="C175" s="4">
-        <v>9127</v>
+        <v>12627</v>
       </c>
       <c r="D175" s="4">
-        <v>4874</v>
+        <v>13417</v>
       </c>
       <c r="E175" s="4">
-        <v>19606</v>
+        <v>21936</v>
       </c>
       <c r="F175" s="4">
-        <v>966</v>
+        <v>943</v>
       </c>
       <c r="G175" s="4">
         <f t="shared" si="2"/>
-        <v>927</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B176" s="4">
-        <v>50294</v>
+        <v>24202</v>
       </c>
       <c r="C176" s="4">
-        <v>12627</v>
+        <v>2872</v>
       </c>
       <c r="D176" s="4">
-        <v>13417</v>
+        <v>18567</v>
       </c>
       <c r="E176" s="4">
-        <v>21936</v>
+        <v>420</v>
       </c>
       <c r="F176" s="4">
-        <v>943</v>
+        <v>1771</v>
       </c>
       <c r="G176" s="4">
         <f t="shared" si="2"/>
-        <v>1371</v>
+        <v>572</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B177" s="4">
-        <v>24202</v>
+        <v>23858</v>
       </c>
       <c r="C177" s="4">
-        <v>2872</v>
+        <v>6357</v>
       </c>
       <c r="D177" s="4">
-        <v>18567</v>
+        <v>6188</v>
       </c>
       <c r="E177" s="4">
-        <v>420</v>
+        <v>7709</v>
       </c>
       <c r="F177" s="4">
-        <v>1771</v>
+        <v>3169</v>
       </c>
       <c r="G177" s="4">
         <f t="shared" si="2"/>
-        <v>572</v>
+        <v>435</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B178" s="4">
-        <v>23858</v>
+        <v>30473</v>
       </c>
       <c r="C178" s="4">
-        <v>6357</v>
+        <v>11744</v>
       </c>
       <c r="D178" s="4">
-        <v>6188</v>
+        <v>7074</v>
       </c>
       <c r="E178" s="4">
-        <v>7709</v>
+        <v>8389</v>
       </c>
       <c r="F178" s="4">
-        <v>3169</v>
+        <v>2409</v>
       </c>
       <c r="G178" s="4">
         <f t="shared" si="2"/>
-        <v>435</v>
+        <v>857</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B179" s="4">
-        <v>30473</v>
+        <v>31214</v>
       </c>
       <c r="C179" s="4">
-        <v>11744</v>
+        <v>8653</v>
       </c>
       <c r="D179" s="4">
-        <v>7074</v>
+        <v>8855</v>
       </c>
       <c r="E179" s="4">
-        <v>8389</v>
+        <v>11426</v>
       </c>
       <c r="F179" s="4">
-        <v>2409</v>
+        <v>1526</v>
       </c>
       <c r="G179" s="4">
         <f t="shared" si="2"/>
-        <v>857</v>
+        <v>754</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B180" s="4">
-        <v>31214</v>
+        <v>19240</v>
       </c>
       <c r="C180" s="4">
-        <v>8653</v>
+        <v>5946</v>
       </c>
       <c r="D180" s="4">
-        <v>8855</v>
+        <v>8117</v>
       </c>
       <c r="E180" s="4">
-        <v>11426</v>
+        <v>3743</v>
       </c>
       <c r="F180" s="4">
-        <v>1526</v>
+        <v>923</v>
       </c>
       <c r="G180" s="4">
         <f t="shared" si="2"/>
-        <v>754</v>
+        <v>511</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B181" s="4">
-        <v>19240</v>
+        <v>18310</v>
       </c>
       <c r="C181" s="4">
-        <v>5946</v>
+        <v>4822</v>
       </c>
       <c r="D181" s="4">
-        <v>8117</v>
+        <v>10585</v>
       </c>
       <c r="E181" s="4">
-        <v>3743</v>
+        <v>1802</v>
       </c>
       <c r="F181" s="4">
-        <v>923</v>
+        <v>723</v>
       </c>
       <c r="G181" s="4">
         <f t="shared" si="2"/>
-        <v>511</v>
+        <v>378</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B182" s="4">
-        <v>18310</v>
+        <v>25635</v>
       </c>
       <c r="C182" s="4">
-        <v>4822</v>
+        <v>7541</v>
       </c>
       <c r="D182" s="4">
-        <v>10585</v>
+        <v>9994</v>
       </c>
       <c r="E182" s="4">
-        <v>1802</v>
+        <v>4825</v>
       </c>
       <c r="F182" s="4">
-        <v>723</v>
+        <v>2780</v>
       </c>
       <c r="G182" s="4">
         <f t="shared" si="2"/>
-        <v>378</v>
+        <v>495</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B183" s="4">
-        <v>25635</v>
+        <v>39517</v>
       </c>
       <c r="C183" s="4">
-        <v>7541</v>
+        <v>5772</v>
       </c>
       <c r="D183" s="4">
-        <v>9994</v>
+        <v>25269</v>
       </c>
       <c r="E183" s="4">
-        <v>4825</v>
+        <v>1489</v>
       </c>
       <c r="F183" s="4">
-        <v>2780</v>
+        <v>6586</v>
       </c>
       <c r="G183" s="4">
         <f t="shared" si="2"/>
-        <v>495</v>
+        <v>401</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B184" s="4">
-        <v>39517</v>
+        <v>14775</v>
       </c>
       <c r="C184" s="4">
-        <v>5772</v>
+        <v>1763</v>
       </c>
       <c r="D184" s="4">
-        <v>25269</v>
+        <v>10562</v>
       </c>
       <c r="E184" s="4">
-        <v>1489</v>
+        <v>728</v>
       </c>
       <c r="F184" s="4">
-        <v>6586</v>
+        <v>1594</v>
       </c>
       <c r="G184" s="4">
         <f t="shared" si="2"/>
-        <v>401</v>
+        <v>128</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B185" s="4">
-        <v>14775</v>
+        <v>31931</v>
       </c>
       <c r="C185" s="4">
-        <v>1763</v>
+        <v>2935</v>
       </c>
       <c r="D185" s="4">
-        <v>10562</v>
+        <v>23711</v>
       </c>
       <c r="E185" s="4">
-        <v>728</v>
+        <v>811</v>
       </c>
       <c r="F185" s="4">
-        <v>1594</v>
+        <v>4206</v>
       </c>
       <c r="G185" s="4">
         <f t="shared" si="2"/>
-        <v>128</v>
+        <v>268</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B186" s="4">
-        <v>31931</v>
+        <v>24999</v>
       </c>
       <c r="C186" s="4">
-        <v>2935</v>
+        <v>3465</v>
       </c>
       <c r="D186" s="4">
-        <v>23711</v>
+        <v>17908</v>
       </c>
       <c r="E186" s="4">
-        <v>811</v>
+        <v>1012</v>
       </c>
       <c r="F186" s="4">
-        <v>4206</v>
+        <v>2187</v>
       </c>
       <c r="G186" s="4">
         <f t="shared" si="2"/>
-        <v>268</v>
+        <v>427</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B187" s="4">
-        <v>24999</v>
+        <v>21208</v>
       </c>
       <c r="C187" s="4">
-        <v>3465</v>
+        <v>3054</v>
       </c>
       <c r="D187" s="4">
-        <v>17908</v>
+        <v>16489</v>
       </c>
       <c r="E187" s="4">
-        <v>1012</v>
+        <v>390</v>
       </c>
       <c r="F187" s="4">
-        <v>2187</v>
+        <v>1123</v>
       </c>
       <c r="G187" s="4">
         <f t="shared" si="2"/>
-        <v>427</v>
+        <v>152</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B188" s="4">
-        <v>21208</v>
+        <v>28727</v>
       </c>
       <c r="C188" s="4">
-        <v>3054</v>
+        <v>2393</v>
       </c>
       <c r="D188" s="4">
-        <v>16489</v>
+        <v>25068</v>
       </c>
       <c r="E188" s="4">
-        <v>390</v>
+        <v>96</v>
       </c>
       <c r="F188" s="4">
-        <v>1123</v>
+        <v>942</v>
       </c>
       <c r="G188" s="4">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>228</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B189" s="4">
-        <v>28727</v>
+        <v>24083</v>
       </c>
       <c r="C189" s="4">
-        <v>2393</v>
+        <v>2969</v>
       </c>
       <c r="D189" s="4">
-        <v>25068</v>
+        <v>18965</v>
       </c>
       <c r="E189" s="4">
-        <v>96</v>
+        <v>711</v>
       </c>
       <c r="F189" s="4">
-        <v>942</v>
+        <v>1044</v>
       </c>
       <c r="G189" s="4">
         <f t="shared" si="2"/>
-        <v>228</v>
+        <v>394</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B190" s="4">
-        <v>24083</v>
+        <v>22038</v>
       </c>
       <c r="C190" s="4">
-        <v>2969</v>
+        <v>2686</v>
       </c>
       <c r="D190" s="4">
-        <v>18965</v>
+        <v>18091</v>
       </c>
       <c r="E190" s="4">
-        <v>711</v>
+        <v>539</v>
       </c>
       <c r="F190" s="4">
-        <v>1044</v>
+        <v>463</v>
       </c>
       <c r="G190" s="4">
         <f t="shared" si="2"/>
-        <v>394</v>
+        <v>259</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B191" s="4">
-        <v>22038</v>
+        <v>19938</v>
       </c>
       <c r="C191" s="4">
-        <v>2686</v>
+        <v>1450</v>
       </c>
       <c r="D191" s="4">
-        <v>18091</v>
+        <v>17137</v>
       </c>
       <c r="E191" s="4">
-        <v>539</v>
+        <v>111</v>
       </c>
       <c r="F191" s="4">
-        <v>463</v>
+        <v>1105</v>
       </c>
       <c r="G191" s="4">
         <f t="shared" si="2"/>
-        <v>259</v>
+        <v>135</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B192" s="4">
-        <v>19938</v>
+        <v>24799</v>
       </c>
       <c r="C192" s="4">
-        <v>1450</v>
+        <v>2848</v>
       </c>
       <c r="D192" s="4">
-        <v>17137</v>
+        <v>19872</v>
       </c>
       <c r="E192" s="4">
-        <v>111</v>
+        <v>400</v>
       </c>
       <c r="F192" s="4">
-        <v>1105</v>
+        <v>1558</v>
       </c>
       <c r="G192" s="4">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B193" s="4">
-        <v>24799</v>
+        <v>43427</v>
       </c>
       <c r="C193" s="4">
-        <v>2848</v>
+        <v>3169</v>
       </c>
       <c r="D193" s="4">
-        <v>19872</v>
+        <v>38133</v>
       </c>
       <c r="E193" s="4">
-        <v>400</v>
+        <v>64</v>
       </c>
       <c r="F193" s="4">
-        <v>1558</v>
+        <v>1664</v>
       </c>
       <c r="G193" s="4">
-        <f t="shared" si="2"/>
-        <v>121</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A194" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B194" s="4">
-        <v>43427</v>
-      </c>
-      <c r="C194" s="4">
-        <v>3169</v>
-      </c>
-      <c r="D194" s="4">
-        <v>38133</v>
-      </c>
-      <c r="E194" s="4">
-        <v>64</v>
-      </c>
-      <c r="F194" s="4">
-        <v>1664</v>
-      </c>
-      <c r="G194" s="4">
-        <f t="shared" ref="G194" si="3">B194-C194-D194-E194-F194</f>
+        <f t="shared" ref="G193" si="3">B193-C193-D193-E193-F193</f>
         <v>397</v>
       </c>
     </row>

</xml_diff>